<commit_message>
adicionando paginas teste da dash
</commit_message>
<xml_diff>
--- a/dashboard/especificacao-dash.xlsx
+++ b/dashboard/especificacao-dash.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/724b8c8d01510d67/Documentos/DATATECH/DataTech-Sprint-2/dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cynth\OneDrive\Documentos\Cynthia\Faculdade\PI\DataTech-Sprint-2\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA678A2-E897-4101-9E83-EF249542DA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BC26B9-EC86-4D09-BD6E-5BAF8506CE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{9504D507-3B1B-4BA3-8A27-5C4284C0FF3F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9504D507-3B1B-4BA3-8A27-5C4284C0FF3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="2" r:id="rId1"/>
@@ -523,6 +523,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,40 +577,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -616,28 +628,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -751,8 +751,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.9075561252077784E-2"/>
-          <c:y val="0.12015606821902962"/>
+          <c:x val="4.2915972525208672E-2"/>
+          <c:y val="0.10019344346127569"/>
           <c:w val="0.96239761280115355"/>
           <c:h val="0.69383423226400398"/>
         </c:manualLayout>
@@ -5059,13 +5059,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1618</xdr:colOff>
+      <xdr:colOff>1617</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>170159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>891049</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>20484</xdr:rowOff>
     </xdr:to>
@@ -5420,17 +5420,17 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
@@ -5440,7 +5440,7 @@
       </c>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>11</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>13</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>14</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>15</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>16</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>17</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>18</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>19</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>20</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>21</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>22</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>23</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>24</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>15</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D30" s="13" t="s">
         <v>7</v>
       </c>
@@ -6080,7 +6080,7 @@
       </c>
       <c r="G30" s="13"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>0</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>1</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>2</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>3</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>4</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>5</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>6</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>7</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>8</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>9</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>10</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>11</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>12</v>
       </c>
@@ -6358,380 +6358,390 @@
   <dimension ref="A2:R77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="P18" sqref="O3:P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="2.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="2.36328125" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" customWidth="1"/>
-    <col min="11" max="14" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="2.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="14" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I3" s="36" t="s">
+    <row r="2" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="37"/>
-    </row>
-    <row r="4" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-    </row>
-    <row r="5" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I5" s="32" t="s">
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
+    </row>
+    <row r="5" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I6" s="32"/>
-      <c r="J6" s="33"/>
-    </row>
-    <row r="7" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I7" s="32"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I9" s="32"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I10" s="34"/>
-      <c r="J10" s="35"/>
-    </row>
-    <row r="13" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I14" s="36" t="s">
+      <c r="J5" s="37"/>
+    </row>
+    <row r="6" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+    </row>
+    <row r="8" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I8" s="36"/>
+      <c r="J8" s="37"/>
+    </row>
+    <row r="9" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+    </row>
+    <row r="13" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I14" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
-    </row>
-    <row r="16" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I16" s="40">
+      <c r="J14" s="41"/>
+    </row>
+    <row r="15" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I15" s="42"/>
+      <c r="J15" s="43"/>
+    </row>
+    <row r="16" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I16" s="44">
         <v>0.65</v>
       </c>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="I17" s="32"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="I18" s="32"/>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="I19" s="32"/>
-      <c r="J19" s="33"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="I20" s="32"/>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
-    </row>
-    <row r="24" spans="1:18" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I20" s="36"/>
+      <c r="J20" s="37"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="38"/>
+      <c r="J21" s="39"/>
+    </row>
+    <row r="24" spans="1:18" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="D25" s="49" t="s">
+      <c r="B25" s="15"/>
+      <c r="D25" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="49" t="s">
+      <c r="E25" s="33"/>
+      <c r="F25" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="50"/>
-      <c r="I25" s="41" t="s">
+      <c r="G25" s="33"/>
+      <c r="I25" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="42"/>
-    </row>
-    <row r="26" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="52"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="44"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="28" t="s">
+      <c r="J25" s="46"/>
+    </row>
+    <row r="26" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="35"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="D27" s="14" t="s">
+      <c r="B27" s="50"/>
+      <c r="D27" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="14" t="s">
+      <c r="E27" s="27"/>
+      <c r="F27" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="I27" s="45" t="s">
+      <c r="G27" s="27"/>
+      <c r="I27" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J27" s="46"/>
+      <c r="J27" s="19"/>
       <c r="R27" s="11"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="46"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="46"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="46"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="46"/>
-    </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="19"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="48"/>
-    </row>
-    <row r="33" spans="1:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="49"/>
+      <c r="B28" s="50"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="50"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="50"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="19"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+      <c r="B31" s="50"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="19"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="51"/>
+      <c r="B32" s="52"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="1:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="21"/>
-    </row>
-    <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23"/>
-    </row>
-    <row r="36" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="24">
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="17"/>
+    </row>
+    <row r="36" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22">
         <v>10</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="23"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
+    <row r="37" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
       <c r="K37" s="8"/>
     </row>
-    <row r="38" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
+    <row r="38" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
+    <row r="39" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22"/>
+      <c r="B39" s="23"/>
       <c r="K39" s="9"/>
     </row>
-    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
+    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="26"/>
-      <c r="B41" s="27"/>
+    <row r="41" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="24"/>
+      <c r="B41" s="25"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="1:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I42" s="8"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="20" t="s">
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="15"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="22"/>
-      <c r="B44" s="23"/>
-    </row>
-    <row r="45" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="28" t="s">
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+    </row>
+    <row r="45" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="29"/>
+      <c r="B45" s="50"/>
       <c r="K45" s="8"/>
     </row>
-    <row r="46" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="28"/>
-      <c r="B46" s="29"/>
+    <row r="46" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
       <c r="K46" s="8"/>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="28"/>
-      <c r="B47" s="29"/>
+    <row r="47" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="49"/>
+      <c r="B47" s="50"/>
       <c r="K47" s="9"/>
       <c r="L47" s="10"/>
     </row>
-    <row r="48" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28"/>
-      <c r="B48" s="29"/>
+    <row r="48" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="49"/>
+      <c r="B48" s="50"/>
       <c r="K48" s="9"/>
       <c r="L48" s="10"/>
     </row>
-    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="28"/>
-      <c r="B49" s="29"/>
+    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="49"/>
+      <c r="B49" s="50"/>
       <c r="K49" s="9"/>
       <c r="L49" s="10"/>
     </row>
-    <row r="50" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="30"/>
-      <c r="B50" s="31"/>
+    <row r="50" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="51"/>
+      <c r="B50" s="52"/>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
     </row>
-    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="20" t="s">
+    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="21"/>
+      <c r="B52" s="15"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="22"/>
-      <c r="B53" s="23"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" s="24">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="16"/>
+      <c r="B53" s="17"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="22">
         <v>7</v>
       </c>
-      <c r="B54" s="25"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" s="24"/>
-      <c r="B55" s="25"/>
+      <c r="B54" s="23"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="22"/>
+      <c r="B55" s="23"/>
       <c r="N55" s="11"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A56" s="24"/>
-      <c r="B56" s="25"/>
-    </row>
-    <row r="57" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="24"/>
-      <c r="B57" s="25"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="22"/>
+      <c r="B56" s="23"/>
+    </row>
+    <row r="57" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="22"/>
+      <c r="B57" s="23"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="24"/>
-      <c r="B58" s="25"/>
+    <row r="58" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="22"/>
+      <c r="B58" s="23"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="26"/>
-      <c r="B59" s="27"/>
+    <row r="59" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="24"/>
+      <c r="B59" s="25"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H61" s="4"/>
     </row>
-    <row r="65" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H70" s="1"/>
     </row>
-    <row r="73" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H74" s="7"/>
     </row>
-    <row r="75" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H75" s="7"/>
     </row>
-    <row r="76" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H76" s="7"/>
     </row>
-    <row r="77" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H77" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="A54:B59"/>
+    <mergeCell ref="A45:B50"/>
+    <mergeCell ref="A27:B32"/>
+    <mergeCell ref="I5:J10"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="I16:J21"/>
+    <mergeCell ref="I25:J26"/>
     <mergeCell ref="A25:B26"/>
     <mergeCell ref="I27:J32"/>
     <mergeCell ref="A34:B35"/>
@@ -6739,17 +6749,7 @@
     <mergeCell ref="D27:E32"/>
     <mergeCell ref="D25:E26"/>
     <mergeCell ref="F25:G26"/>
-    <mergeCell ref="I5:J10"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="I16:J21"/>
-    <mergeCell ref="I25:J26"/>
     <mergeCell ref="F27:G32"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="A54:B59"/>
-    <mergeCell ref="A45:B50"/>
-    <mergeCell ref="A27:B32"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -6757,12 +6757,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="90fcf95d-5720-49ef-8433-32c5e8162615">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6985,19 +6986,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="90fcf95d-5720-49ef-8433-32c5e8162615">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{644901F6-D494-434C-8948-F604DCF7F096}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03ADDD95-D2F0-4266-A4B5-2CD0720E3AA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="90fcf95d-5720-49ef-8433-32c5e8162615"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7022,11 +7024,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03ADDD95-D2F0-4266-A4B5-2CD0720E3AA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{644901F6-D494-434C-8948-F604DCF7F096}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="90fcf95d-5720-49ef-8433-32c5e8162615"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>